<commit_message>
my assignment 2 plus combo firearms data
</commit_message>
<xml_diff>
--- a/data/Firearms Manufactured 1990-2016.xlsx
+++ b/data/Firearms Manufactured 1990-2016.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rayxiao/GitHub/berkeley/W209/w209_final_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DD371183-E01F-5140-88DB-39A4A9E2D69D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589368D5-148F-CE43-B76E-24654D173052}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Firearms Manufactured 1990-2016" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Calendar Total Year</t>
-  </si>
   <si>
     <t>Pistols</t>
   </si>
@@ -40,13 +37,16 @@
     <t>Misc. Firearms</t>
   </si>
   <si>
-    <t>Firearms</t>
+    <t>Calendar Year</t>
+  </si>
+  <si>
+    <t>Total Firearms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -881,7 +881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -890,22 +890,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>

</xml_diff>